<commit_message>
more updates to database, linkage of database to html
</commit_message>
<xml_diff>
--- a/Booking Room Database/bookingRoom_database.xlsx
+++ b/Booking Room Database/bookingRoom_database.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\invertedsky\Downloads\UOW Com Sci\term4 Oct - Dec 2022\CSIT214 - IT Project Management\CSIT214 Github\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\invertedsky\Downloads\UOW Com Sci\term4 Oct - Dec 2022\CSIT214 - IT Project Management\CSIT214 Github\Booking Room Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3CFA2CC-7351-47B6-AAF6-40F6CC4B797A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{530B5AAB-66C7-4C1C-BC95-B34F991103CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7118D649-F7F4-43F0-96A9-F1B2507B603A}"/>
+    <workbookView xWindow="5160" yWindow="1665" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{7118D649-F7F4-43F0-96A9-F1B2507B603A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Lists of Rooms available" sheetId="1" r:id="rId1"/>
-    <sheet name="Launched Rooms" sheetId="2" r:id="rId2"/>
+    <sheet name="ListOfRooms_Staff" sheetId="1" r:id="rId1"/>
+    <sheet name="ListOfRooms_Student" sheetId="3" r:id="rId2"/>
+    <sheet name="Launched Rooms" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="53">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -193,6 +194,9 @@
   </si>
   <si>
     <t>UI786</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -316,7 +320,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -344,13 +348,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -367,6 +368,33 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -683,8 +711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7059910A-97E4-4DFA-82E8-B2360B706696}">
   <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -756,16 +784,16 @@
         <f>C2+2*(1/24)</f>
         <v>0.41666666666666663</v>
       </c>
-      <c r="D3" s="13">
-        <v>8</v>
-      </c>
-      <c r="E3" s="13">
+      <c r="D3" s="3">
+        <v>8</v>
+      </c>
+      <c r="E3" s="3">
         <v>11</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="14">
+      <c r="G3" s="13">
         <v>5</v>
       </c>
     </row>
@@ -781,16 +809,16 @@
         <f t="shared" ref="C4:C22" si="1">C3+2*(1/24)</f>
         <v>0.49999999999999994</v>
       </c>
-      <c r="D4" s="13">
-        <v>8</v>
-      </c>
-      <c r="E4" s="13">
+      <c r="D4" s="3">
+        <v>8</v>
+      </c>
+      <c r="E4" s="3">
         <v>28</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="14">
+      <c r="G4" s="13">
         <v>15</v>
       </c>
     </row>
@@ -806,16 +834,16 @@
         <f t="shared" si="1"/>
         <v>0.58333333333333326</v>
       </c>
-      <c r="D5" s="13">
-        <v>8</v>
-      </c>
-      <c r="E5" s="13">
-        <v>20</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="14">
+      <c r="D5" s="3">
+        <v>8</v>
+      </c>
+      <c r="E5" s="3">
+        <v>20</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="13">
         <v>5</v>
       </c>
     </row>
@@ -831,16 +859,16 @@
         <f t="shared" si="1"/>
         <v>0.66666666666666663</v>
       </c>
-      <c r="D6" s="13">
-        <v>8</v>
-      </c>
-      <c r="E6" s="13">
+      <c r="D6" s="3">
+        <v>8</v>
+      </c>
+      <c r="E6" s="3">
         <v>10</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="13">
         <v>10</v>
       </c>
     </row>
@@ -856,16 +884,16 @@
         <f t="shared" si="1"/>
         <v>0.75</v>
       </c>
-      <c r="D7" s="13">
-        <v>8</v>
-      </c>
-      <c r="E7" s="13">
+      <c r="D7" s="3">
+        <v>8</v>
+      </c>
+      <c r="E7" s="3">
         <v>26</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="14">
+      <c r="G7" s="13">
         <v>5</v>
       </c>
     </row>
@@ -881,16 +909,16 @@
         <f t="shared" si="1"/>
         <v>0.83333333333333337</v>
       </c>
-      <c r="D8" s="13">
-        <v>8</v>
-      </c>
-      <c r="E8" s="13">
+      <c r="D8" s="3">
+        <v>8</v>
+      </c>
+      <c r="E8" s="3">
         <v>22</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="14">
+      <c r="G8" s="13">
         <v>5</v>
       </c>
     </row>
@@ -929,16 +957,16 @@
       <c r="C10" s="12">
         <v>0.41666666666666663</v>
       </c>
-      <c r="D10" s="13">
-        <v>50</v>
-      </c>
-      <c r="E10" s="13">
+      <c r="D10" s="3">
+        <v>50</v>
+      </c>
+      <c r="E10" s="3">
         <v>12</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="F10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="14">
+      <c r="G10" s="13">
         <v>5</v>
       </c>
     </row>
@@ -953,16 +981,16 @@
       <c r="C11" s="12">
         <v>0.49999999999999994</v>
       </c>
-      <c r="D11" s="13">
-        <v>50</v>
-      </c>
-      <c r="E11" s="13">
+      <c r="D11" s="3">
+        <v>50</v>
+      </c>
+      <c r="E11" s="3">
         <v>29</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="F11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="14">
+      <c r="G11" s="13">
         <v>10</v>
       </c>
     </row>
@@ -977,16 +1005,16 @@
       <c r="C12" s="12">
         <v>0.58333333333333326</v>
       </c>
-      <c r="D12" s="13">
-        <v>50</v>
-      </c>
-      <c r="E12" s="13">
+      <c r="D12" s="3">
+        <v>50</v>
+      </c>
+      <c r="E12" s="3">
         <v>23</v>
       </c>
-      <c r="F12" s="13" t="s">
+      <c r="F12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="14">
+      <c r="G12" s="13">
         <v>10</v>
       </c>
     </row>
@@ -1001,16 +1029,16 @@
       <c r="C13" s="12">
         <v>0.66666666666666663</v>
       </c>
-      <c r="D13" s="13">
-        <v>50</v>
-      </c>
-      <c r="E13" s="13">
+      <c r="D13" s="3">
+        <v>50</v>
+      </c>
+      <c r="E13" s="3">
         <v>10</v>
       </c>
-      <c r="F13" s="13" t="s">
+      <c r="F13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="14">
+      <c r="G13" s="13">
         <v>10</v>
       </c>
     </row>
@@ -1025,40 +1053,40 @@
       <c r="C14" s="12">
         <v>0.75</v>
       </c>
-      <c r="D14" s="13">
-        <v>50</v>
-      </c>
-      <c r="E14" s="13">
+      <c r="D14" s="3">
+        <v>50</v>
+      </c>
+      <c r="E14" s="3">
         <v>23</v>
       </c>
-      <c r="F14" s="13" t="s">
+      <c r="F14" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G14" s="14">
+      <c r="G14" s="13">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="B15" s="16">
-        <f t="shared" si="0"/>
-        <v>44854</v>
-      </c>
-      <c r="C15" s="17">
+      <c r="A15" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="15">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="C15" s="16">
         <v>0.83333333333333337</v>
       </c>
-      <c r="D15" s="18">
-        <v>50</v>
-      </c>
-      <c r="E15" s="18">
+      <c r="D15" s="17">
+        <v>50</v>
+      </c>
+      <c r="E15" s="17">
         <v>25</v>
       </c>
-      <c r="F15" s="18" t="s">
+      <c r="F15" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="G15" s="19">
+      <c r="G15" s="18">
         <v>15</v>
       </c>
     </row>
@@ -1098,16 +1126,16 @@
         <f>C16+2*(1/24)</f>
         <v>0.41666666666666663</v>
       </c>
-      <c r="D17" s="13">
-        <v>20</v>
-      </c>
-      <c r="E17" s="13">
+      <c r="D17" s="3">
+        <v>20</v>
+      </c>
+      <c r="E17" s="3">
         <v>29</v>
       </c>
-      <c r="F17" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="G17" s="14">
+      <c r="F17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" s="13">
         <v>10</v>
       </c>
     </row>
@@ -1123,16 +1151,16 @@
         <f t="shared" si="1"/>
         <v>0.49999999999999994</v>
       </c>
-      <c r="D18" s="13">
-        <v>20</v>
-      </c>
-      <c r="E18" s="13">
-        <v>20</v>
-      </c>
-      <c r="F18" s="13" t="s">
+      <c r="D18" s="3">
+        <v>20</v>
+      </c>
+      <c r="E18" s="3">
+        <v>20</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G18" s="14">
+      <c r="G18" s="13">
         <v>5</v>
       </c>
     </row>
@@ -1148,16 +1176,16 @@
         <f t="shared" si="1"/>
         <v>0.58333333333333326</v>
       </c>
-      <c r="D19" s="13">
-        <v>20</v>
-      </c>
-      <c r="E19" s="13">
+      <c r="D19" s="3">
+        <v>20</v>
+      </c>
+      <c r="E19" s="3">
         <v>16</v>
       </c>
-      <c r="F19" s="13" t="s">
+      <c r="F19" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G19" s="14">
+      <c r="G19" s="13">
         <v>15</v>
       </c>
     </row>
@@ -1173,16 +1201,16 @@
         <f t="shared" si="1"/>
         <v>0.66666666666666663</v>
       </c>
-      <c r="D20" s="13">
-        <v>20</v>
-      </c>
-      <c r="E20" s="13">
+      <c r="D20" s="3">
+        <v>20</v>
+      </c>
+      <c r="E20" s="3">
         <v>24</v>
       </c>
-      <c r="F20" s="13" t="s">
+      <c r="F20" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G20" s="14">
+      <c r="G20" s="13">
         <v>10</v>
       </c>
     </row>
@@ -1198,41 +1226,41 @@
         <f t="shared" si="1"/>
         <v>0.75</v>
       </c>
-      <c r="D21" s="13">
-        <v>20</v>
-      </c>
-      <c r="E21" s="13">
+      <c r="D21" s="3">
+        <v>20</v>
+      </c>
+      <c r="E21" s="3">
         <v>27</v>
       </c>
-      <c r="F21" s="13" t="s">
+      <c r="F21" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G21" s="14">
+      <c r="G21" s="13">
         <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="B22" s="16">
-        <f t="shared" si="0"/>
-        <v>44854</v>
-      </c>
-      <c r="C22" s="17">
+      <c r="A22" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="15">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="C22" s="16">
         <f t="shared" si="1"/>
         <v>0.83333333333333337</v>
       </c>
-      <c r="D22" s="18">
-        <v>20</v>
-      </c>
-      <c r="E22" s="18">
-        <v>20</v>
-      </c>
-      <c r="F22" s="18" t="s">
+      <c r="D22" s="17">
+        <v>20</v>
+      </c>
+      <c r="E22" s="17">
+        <v>20</v>
+      </c>
+      <c r="F22" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="G22" s="19">
+      <c r="G22" s="18">
         <v>5</v>
       </c>
     </row>
@@ -1272,16 +1300,16 @@
         <f>C23+2*(1/24)</f>
         <v>0.41666666666666663</v>
       </c>
-      <c r="D24" s="13">
-        <v>8</v>
-      </c>
-      <c r="E24" s="13">
+      <c r="D24" s="3">
+        <v>8</v>
+      </c>
+      <c r="E24" s="3">
         <v>13</v>
       </c>
-      <c r="F24" s="13" t="s">
+      <c r="F24" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G24" s="14">
+      <c r="G24" s="13">
         <v>10</v>
       </c>
     </row>
@@ -1294,19 +1322,19 @@
         <v>44854</v>
       </c>
       <c r="C25" s="12">
-        <f t="shared" ref="C25:C43" si="2">C24+2*(1/24)</f>
+        <f t="shared" ref="C25:C29" si="2">C24+2*(1/24)</f>
         <v>0.49999999999999994</v>
       </c>
-      <c r="D25" s="13">
-        <v>8</v>
-      </c>
-      <c r="E25" s="13">
+      <c r="D25" s="3">
+        <v>8</v>
+      </c>
+      <c r="E25" s="3">
         <v>16</v>
       </c>
-      <c r="F25" s="13" t="s">
+      <c r="F25" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G25" s="14">
+      <c r="G25" s="13">
         <v>5</v>
       </c>
     </row>
@@ -1322,16 +1350,16 @@
         <f t="shared" si="2"/>
         <v>0.58333333333333326</v>
       </c>
-      <c r="D26" s="13">
-        <v>8</v>
-      </c>
-      <c r="E26" s="13">
+      <c r="D26" s="3">
+        <v>8</v>
+      </c>
+      <c r="E26" s="3">
         <v>11</v>
       </c>
-      <c r="F26" s="13" t="s">
+      <c r="F26" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G26" s="14">
+      <c r="G26" s="13">
         <v>5</v>
       </c>
     </row>
@@ -1347,16 +1375,16 @@
         <f t="shared" si="2"/>
         <v>0.66666666666666663</v>
       </c>
-      <c r="D27" s="13">
-        <v>8</v>
-      </c>
-      <c r="E27" s="13">
+      <c r="D27" s="3">
+        <v>8</v>
+      </c>
+      <c r="E27" s="3">
         <v>19</v>
       </c>
-      <c r="F27" s="13" t="s">
+      <c r="F27" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G27" s="14">
+      <c r="G27" s="13">
         <v>10</v>
       </c>
     </row>
@@ -1372,41 +1400,41 @@
         <f t="shared" si="2"/>
         <v>0.75</v>
       </c>
-      <c r="D28" s="13">
-        <v>8</v>
-      </c>
-      <c r="E28" s="13">
+      <c r="D28" s="3">
+        <v>8</v>
+      </c>
+      <c r="E28" s="3">
         <v>13</v>
       </c>
-      <c r="F28" s="13" t="s">
+      <c r="F28" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G28" s="14">
+      <c r="G28" s="13">
         <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="B29" s="16">
-        <f t="shared" si="0"/>
-        <v>44854</v>
-      </c>
-      <c r="C29" s="17">
+      <c r="A29" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" s="15">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="C29" s="16">
         <f t="shared" si="2"/>
         <v>0.83333333333333337</v>
       </c>
-      <c r="D29" s="18">
-        <v>8</v>
-      </c>
-      <c r="E29" s="18">
+      <c r="D29" s="17">
+        <v>8</v>
+      </c>
+      <c r="E29" s="17">
         <v>15</v>
       </c>
-      <c r="F29" s="18" t="s">
+      <c r="F29" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="G29" s="19">
+      <c r="G29" s="18">
         <v>5</v>
       </c>
     </row>
@@ -1445,16 +1473,16 @@
       <c r="C31" s="12">
         <v>0.41666666666666663</v>
       </c>
-      <c r="D31" s="13">
-        <v>50</v>
-      </c>
-      <c r="E31" s="13">
+      <c r="D31" s="3">
+        <v>50</v>
+      </c>
+      <c r="E31" s="3">
         <v>15</v>
       </c>
-      <c r="F31" s="13" t="s">
+      <c r="F31" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G31" s="14">
+      <c r="G31" s="13">
         <v>5</v>
       </c>
     </row>
@@ -1469,16 +1497,16 @@
       <c r="C32" s="12">
         <v>0.49999999999999994</v>
       </c>
-      <c r="D32" s="13">
-        <v>50</v>
-      </c>
-      <c r="E32" s="13">
-        <v>20</v>
-      </c>
-      <c r="F32" s="13" t="s">
+      <c r="D32" s="3">
+        <v>50</v>
+      </c>
+      <c r="E32" s="3">
+        <v>20</v>
+      </c>
+      <c r="F32" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G32" s="14">
+      <c r="G32" s="13">
         <v>5</v>
       </c>
     </row>
@@ -1493,16 +1521,16 @@
       <c r="C33" s="12">
         <v>0.58333333333333326</v>
       </c>
-      <c r="D33" s="13">
-        <v>50</v>
-      </c>
-      <c r="E33" s="13">
+      <c r="D33" s="3">
+        <v>50</v>
+      </c>
+      <c r="E33" s="3">
         <v>24</v>
       </c>
-      <c r="F33" s="13" t="s">
+      <c r="F33" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G33" s="14">
+      <c r="G33" s="13">
         <v>10</v>
       </c>
     </row>
@@ -1517,16 +1545,16 @@
       <c r="C34" s="12">
         <v>0.66666666666666663</v>
       </c>
-      <c r="D34" s="13">
-        <v>50</v>
-      </c>
-      <c r="E34" s="13">
+      <c r="D34" s="3">
+        <v>50</v>
+      </c>
+      <c r="E34" s="3">
         <v>28</v>
       </c>
-      <c r="F34" s="13" t="s">
+      <c r="F34" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G34" s="14">
+      <c r="G34" s="13">
         <v>15</v>
       </c>
     </row>
@@ -1541,40 +1569,40 @@
       <c r="C35" s="12">
         <v>0.75</v>
       </c>
-      <c r="D35" s="13">
-        <v>50</v>
-      </c>
-      <c r="E35" s="13">
+      <c r="D35" s="3">
+        <v>50</v>
+      </c>
+      <c r="E35" s="3">
         <v>28</v>
       </c>
-      <c r="F35" s="13" t="s">
+      <c r="F35" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G35" s="14">
+      <c r="G35" s="13">
         <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="B36" s="16">
-        <f t="shared" si="0"/>
-        <v>44854</v>
-      </c>
-      <c r="C36" s="17">
+      <c r="A36" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36" s="15">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="C36" s="16">
         <v>0.83333333333333337</v>
       </c>
-      <c r="D36" s="18">
-        <v>50</v>
-      </c>
-      <c r="E36" s="18">
+      <c r="D36" s="17">
+        <v>50</v>
+      </c>
+      <c r="E36" s="17">
         <v>17</v>
       </c>
-      <c r="F36" s="18" t="s">
+      <c r="F36" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="G36" s="19">
+      <c r="G36" s="18">
         <v>5</v>
       </c>
     </row>
@@ -1614,16 +1642,16 @@
         <f>C37+2*(1/24)</f>
         <v>0.41666666666666663</v>
       </c>
-      <c r="D38" s="13">
-        <v>20</v>
-      </c>
-      <c r="E38" s="13">
+      <c r="D38" s="3">
+        <v>20</v>
+      </c>
+      <c r="E38" s="3">
         <v>28</v>
       </c>
-      <c r="F38" s="13" t="s">
+      <c r="F38" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G38" s="14">
+      <c r="G38" s="13">
         <v>10</v>
       </c>
     </row>
@@ -1639,16 +1667,16 @@
         <f t="shared" ref="C39:C43" si="3">C38+2*(1/24)</f>
         <v>0.49999999999999994</v>
       </c>
-      <c r="D39" s="13">
-        <v>20</v>
-      </c>
-      <c r="E39" s="13">
+      <c r="D39" s="3">
+        <v>20</v>
+      </c>
+      <c r="E39" s="3">
         <v>13</v>
       </c>
-      <c r="F39" s="13" t="s">
+      <c r="F39" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G39" s="14">
+      <c r="G39" s="13">
         <v>15</v>
       </c>
     </row>
@@ -1664,16 +1692,16 @@
         <f t="shared" si="3"/>
         <v>0.58333333333333326</v>
       </c>
-      <c r="D40" s="13">
-        <v>20</v>
-      </c>
-      <c r="E40" s="13">
+      <c r="D40" s="3">
+        <v>20</v>
+      </c>
+      <c r="E40" s="3">
         <v>13</v>
       </c>
-      <c r="F40" s="13" t="s">
+      <c r="F40" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G40" s="14">
+      <c r="G40" s="13">
         <v>5</v>
       </c>
     </row>
@@ -1689,16 +1717,16 @@
         <f t="shared" si="3"/>
         <v>0.66666666666666663</v>
       </c>
-      <c r="D41" s="13">
-        <v>20</v>
-      </c>
-      <c r="E41" s="13">
+      <c r="D41" s="3">
+        <v>20</v>
+      </c>
+      <c r="E41" s="3">
         <v>26</v>
       </c>
-      <c r="F41" s="13" t="s">
+      <c r="F41" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="G41" s="14">
+      <c r="G41" s="13">
         <v>15</v>
       </c>
     </row>
@@ -1714,41 +1742,41 @@
         <f t="shared" si="3"/>
         <v>0.75</v>
       </c>
-      <c r="D42" s="13">
-        <v>20</v>
-      </c>
-      <c r="E42" s="13">
+      <c r="D42" s="3">
+        <v>20</v>
+      </c>
+      <c r="E42" s="3">
         <v>11</v>
       </c>
-      <c r="F42" s="13" t="s">
+      <c r="F42" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="G42" s="14">
+      <c r="G42" s="13">
         <v>20</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="B43" s="16">
-        <f t="shared" si="0"/>
-        <v>44854</v>
-      </c>
-      <c r="C43" s="17">
+      <c r="A43" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B43" s="15">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="C43" s="16">
         <f t="shared" si="3"/>
         <v>0.83333333333333337</v>
       </c>
-      <c r="D43" s="18">
-        <v>20</v>
-      </c>
-      <c r="E43" s="18">
-        <v>20</v>
-      </c>
-      <c r="F43" s="18" t="s">
+      <c r="D43" s="17">
+        <v>20</v>
+      </c>
+      <c r="E43" s="17">
+        <v>20</v>
+      </c>
+      <c r="F43" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="G43" s="19">
+      <c r="G43" s="18">
         <v>10</v>
       </c>
     </row>
@@ -1759,6 +1787,698 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C4ED15D-191C-4AAB-A5B7-A6DBCC742E4E}">
+  <dimension ref="A1:L43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17" style="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" style="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="6">
+        <f>DATE(2022,10,20)</f>
+        <v>44854</v>
+      </c>
+      <c r="C2" s="7">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D2" s="22">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="23">
+        <f t="shared" ref="B3:B43" si="0">DATE(2022,10,20)</f>
+        <v>44854</v>
+      </c>
+      <c r="C3" s="24">
+        <f>C2+2*(1/24)</f>
+        <v>0.41666666666666663</v>
+      </c>
+      <c r="D3" s="25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="23">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="C4" s="24">
+        <f t="shared" ref="C4:C22" si="1">C3+2*(1/24)</f>
+        <v>0.49999999999999994</v>
+      </c>
+      <c r="D4" s="25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="23">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="C5" s="24">
+        <f t="shared" si="1"/>
+        <v>0.58333333333333326</v>
+      </c>
+      <c r="D5" s="25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="23">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="C6" s="24">
+        <f t="shared" si="1"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D6" s="25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="23">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="C7" s="24">
+        <f t="shared" si="1"/>
+        <v>0.75</v>
+      </c>
+      <c r="D7" s="25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="23">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="C8" s="24">
+        <f t="shared" si="1"/>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D8" s="25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="6">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="C9" s="7">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D9" s="22">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="23">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="C10" s="24">
+        <v>0.41666666666666663</v>
+      </c>
+      <c r="D10" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="23">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="C11" s="24">
+        <v>0.49999999999999994</v>
+      </c>
+      <c r="D11" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="23">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="C12" s="24">
+        <v>0.58333333333333326</v>
+      </c>
+      <c r="D12" s="25">
+        <v>50</v>
+      </c>
+      <c r="L12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="23">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="C13" s="24">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D13" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="23">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="C14" s="24">
+        <v>0.75</v>
+      </c>
+      <c r="D14" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="15">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="C15" s="16">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D15" s="26">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="6">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="C16" s="7">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D16" s="22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="23">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="C17" s="24">
+        <f>C16+2*(1/24)</f>
+        <v>0.41666666666666663</v>
+      </c>
+      <c r="D17" s="25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="23">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="C18" s="24">
+        <f t="shared" si="1"/>
+        <v>0.49999999999999994</v>
+      </c>
+      <c r="D18" s="25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="23">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="C19" s="24">
+        <f t="shared" si="1"/>
+        <v>0.58333333333333326</v>
+      </c>
+      <c r="D19" s="25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="23">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="C20" s="24">
+        <f t="shared" si="1"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D20" s="25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="23">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="C21" s="24">
+        <f t="shared" si="1"/>
+        <v>0.75</v>
+      </c>
+      <c r="D21" s="25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="15">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="C22" s="16">
+        <f t="shared" si="1"/>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D22" s="26">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="6">
+        <f>DATE(2022,10,20)</f>
+        <v>44854</v>
+      </c>
+      <c r="C23" s="7">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D23" s="22">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="23">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="C24" s="24">
+        <f>C23+2*(1/24)</f>
+        <v>0.41666666666666663</v>
+      </c>
+      <c r="D24" s="25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="23">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="C25" s="24">
+        <f t="shared" ref="C25:C29" si="2">C24+2*(1/24)</f>
+        <v>0.49999999999999994</v>
+      </c>
+      <c r="D25" s="25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" s="23">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="C26" s="24">
+        <f t="shared" si="2"/>
+        <v>0.58333333333333326</v>
+      </c>
+      <c r="D26" s="25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" s="23">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="C27" s="24">
+        <f t="shared" si="2"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D27" s="25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" s="23">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="C28" s="24">
+        <f t="shared" si="2"/>
+        <v>0.75</v>
+      </c>
+      <c r="D28" s="25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" s="15">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="C29" s="16">
+        <f t="shared" si="2"/>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D29" s="26">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="6">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="C30" s="7">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D30" s="22">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" s="23">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="C31" s="24">
+        <v>0.41666666666666663</v>
+      </c>
+      <c r="D31" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" s="23">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="C32" s="24">
+        <v>0.49999999999999994</v>
+      </c>
+      <c r="D32" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" s="23">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="C33" s="24">
+        <v>0.58333333333333326</v>
+      </c>
+      <c r="D33" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B34" s="23">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="C34" s="24">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D34" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B35" s="23">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="C35" s="24">
+        <v>0.75</v>
+      </c>
+      <c r="D35" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36" s="15">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="C36" s="16">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D36" s="26">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B37" s="6">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="C37" s="7">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D37" s="22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B38" s="23">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="C38" s="24">
+        <f>C37+2*(1/24)</f>
+        <v>0.41666666666666663</v>
+      </c>
+      <c r="D38" s="25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39" s="23">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="C39" s="24">
+        <f t="shared" ref="C39:C43" si="3">C38+2*(1/24)</f>
+        <v>0.49999999999999994</v>
+      </c>
+      <c r="D39" s="25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B40" s="23">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="C40" s="24">
+        <f t="shared" si="3"/>
+        <v>0.58333333333333326</v>
+      </c>
+      <c r="D40" s="25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B41" s="23">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="C41" s="24">
+        <f t="shared" si="3"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D41" s="25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B42" s="23">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="C42" s="24">
+        <f t="shared" si="3"/>
+        <v>0.75</v>
+      </c>
+      <c r="D42" s="25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B43" s="15">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="C43" s="16">
+        <f t="shared" si="3"/>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D43" s="26">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9E57897-8241-456F-B820-85D5C0044E1A}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
updated word doc to match new requirements (as of 22nd Oct)
</commit_message>
<xml_diff>
--- a/Booking Room Database/bookingRoom_database.xlsx
+++ b/Booking Room Database/bookingRoom_database.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\invertedsky\Downloads\UOW Com Sci\term4 Oct - Dec 2022\CSIT214 - IT Project Management\CSIT214 Github\Booking Room Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE07D722-7639-4396-BE3C-D91AD2BDD7BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AD51459-8685-45A1-AEAE-62897F17DE4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7118D649-F7F4-43F0-96A9-F1B2507B603A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{7118D649-F7F4-43F0-96A9-F1B2507B603A}"/>
   </bookViews>
   <sheets>
-    <sheet name="ListOfRooms_Staff" sheetId="1" r:id="rId1"/>
-    <sheet name="ListOfRooms_Student" sheetId="3" r:id="rId2"/>
-    <sheet name="Launched Rooms" sheetId="2" r:id="rId3"/>
+    <sheet name="Data Overview" sheetId="4" r:id="rId1"/>
+    <sheet name="ListOfRooms_Staff" sheetId="1" r:id="rId2"/>
+    <sheet name="ListOfRooms_Student" sheetId="3" r:id="rId3"/>
+    <sheet name="Launched Rooms" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="50">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -145,10 +146,49 @@
     <t>Animal Kingdom</t>
   </si>
   <si>
-    <t>Savory Food</t>
-  </si>
-  <si>
     <t>Desserts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type of Rooms </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recreation Room </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Room Names </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cupcakes </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ice Cream </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cake </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cookies </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cheetah </t>
+  </si>
+  <si>
+    <t>Lion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monkey </t>
+  </si>
+  <si>
+    <t>Colors</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Green </t>
+  </si>
+  <si>
+    <t xml:space="preserve">White </t>
   </si>
 </sst>
 </file>
@@ -172,15 +212,39 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -268,11 +332,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -332,19 +424,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -658,11 +760,110 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F00E74DC-7539-45C7-B916-FBEA91259C99}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="26"/>
+      <c r="B3" s="32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="26"/>
+      <c r="B4" s="32" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="27"/>
+      <c r="B5" s="33" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="28"/>
+      <c r="B7" s="30" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="28"/>
+      <c r="B8" s="30" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="31" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="29"/>
+      <c r="B10" s="31" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="29"/>
+      <c r="B11" s="31" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A9:A11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7059910A-97E4-4DFA-82E8-B2360B706696}">
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -698,7 +899,7 @@
       <c r="G1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="H1" s="24" t="s">
         <v>26</v>
       </c>
     </row>
@@ -707,7 +908,7 @@
         <v>27</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" s="6">
         <f>DATE(2022,10,20)</f>
@@ -733,24 +934,24 @@
       <c r="A3" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="25">
+      <c r="B3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="11">
         <f t="shared" ref="C3:C22" si="0">DATE(2022,10,20)</f>
         <v>44854</v>
       </c>
-      <c r="D3" s="26">
+      <c r="D3" s="12">
         <f>D2+2*(1/24)</f>
         <v>0.41666666666666663</v>
       </c>
-      <c r="E3" s="23">
+      <c r="E3" s="3">
         <v>8</v>
       </c>
-      <c r="F3" s="23">
+      <c r="F3" s="3">
         <v>11</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="H3" s="13">
@@ -761,24 +962,24 @@
       <c r="A4" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="25">
-        <f t="shared" si="0"/>
-        <v>44854</v>
-      </c>
-      <c r="D4" s="26">
+      <c r="B4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="11">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="D4" s="12">
         <f t="shared" ref="D4:D22" si="1">D3+2*(1/24)</f>
         <v>0.49999999999999994</v>
       </c>
-      <c r="E4" s="23">
+      <c r="E4" s="3">
         <v>8</v>
       </c>
-      <c r="F4" s="23">
+      <c r="F4" s="3">
         <v>28</v>
       </c>
-      <c r="G4" s="23" t="s">
+      <c r="G4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="H4" s="13">
@@ -789,24 +990,24 @@
       <c r="A5" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="25">
-        <f t="shared" si="0"/>
-        <v>44854</v>
-      </c>
-      <c r="D5" s="26">
+      <c r="B5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="11">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="D5" s="12">
         <f t="shared" si="1"/>
         <v>0.58333333333333326</v>
       </c>
-      <c r="E5" s="23">
+      <c r="E5" s="3">
         <v>8</v>
       </c>
-      <c r="F5" s="23">
-        <v>20</v>
-      </c>
-      <c r="G5" s="23" t="s">
+      <c r="F5" s="3">
+        <v>20</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>8</v>
       </c>
       <c r="H5" s="13">
@@ -817,24 +1018,24 @@
       <c r="A6" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" s="25">
-        <f t="shared" si="0"/>
-        <v>44854</v>
-      </c>
-      <c r="D6" s="26">
+      <c r="B6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="11">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="D6" s="12">
         <f t="shared" si="1"/>
         <v>0.66666666666666663</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="3">
         <v>8</v>
       </c>
-      <c r="F6" s="23">
+      <c r="F6" s="3">
         <v>10</v>
       </c>
-      <c r="G6" s="23" t="s">
+      <c r="G6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="H6" s="13">
@@ -845,24 +1046,24 @@
       <c r="A7" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" s="25">
-        <f t="shared" si="0"/>
-        <v>44854</v>
-      </c>
-      <c r="D7" s="26">
+      <c r="B7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="11">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="D7" s="12">
         <f t="shared" si="1"/>
         <v>0.75</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="3">
         <v>8</v>
       </c>
-      <c r="F7" s="23">
+      <c r="F7" s="3">
         <v>26</v>
       </c>
-      <c r="G7" s="23" t="s">
+      <c r="G7" s="3" t="s">
         <v>10</v>
       </c>
       <c r="H7" s="13">
@@ -873,24 +1074,24 @@
       <c r="A8" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" s="25">
-        <f t="shared" si="0"/>
-        <v>44854</v>
-      </c>
-      <c r="D8" s="26">
+      <c r="B8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="11">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="D8" s="12">
         <f t="shared" si="1"/>
         <v>0.83333333333333337</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="3">
         <v>8</v>
       </c>
-      <c r="F8" s="23">
+      <c r="F8" s="3">
         <v>22</v>
       </c>
-      <c r="G8" s="23" t="s">
+      <c r="G8" s="3" t="s">
         <v>11</v>
       </c>
       <c r="H8" s="13">
@@ -928,23 +1129,23 @@
       <c r="A10" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="25">
-        <f t="shared" si="0"/>
-        <v>44854</v>
-      </c>
-      <c r="D10" s="26">
+      <c r="C10" s="11">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="D10" s="12">
         <v>0.41666666666666663</v>
       </c>
-      <c r="E10" s="23">
+      <c r="E10" s="3">
         <v>50</v>
       </c>
-      <c r="F10" s="23">
+      <c r="F10" s="3">
         <v>12</v>
       </c>
-      <c r="G10" s="23" t="s">
+      <c r="G10" s="3" t="s">
         <v>13</v>
       </c>
       <c r="H10" s="13">
@@ -955,23 +1156,23 @@
       <c r="A11" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="25">
-        <f t="shared" si="0"/>
-        <v>44854</v>
-      </c>
-      <c r="D11" s="26">
+      <c r="C11" s="11">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="D11" s="12">
         <v>0.49999999999999994</v>
       </c>
-      <c r="E11" s="23">
+      <c r="E11" s="3">
         <v>50</v>
       </c>
-      <c r="F11" s="23">
-        <v>29</v>
-      </c>
-      <c r="G11" s="23" t="s">
+      <c r="F11" s="3">
+        <v>29</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>14</v>
       </c>
       <c r="H11" s="13">
@@ -982,23 +1183,23 @@
       <c r="A12" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="25">
-        <f t="shared" si="0"/>
-        <v>44854</v>
-      </c>
-      <c r="D12" s="26">
+      <c r="C12" s="11">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="D12" s="12">
         <v>0.58333333333333326</v>
       </c>
-      <c r="E12" s="23">
+      <c r="E12" s="3">
         <v>50</v>
       </c>
-      <c r="F12" s="23">
+      <c r="F12" s="3">
         <v>23</v>
       </c>
-      <c r="G12" s="23" t="s">
+      <c r="G12" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H12" s="13">
@@ -1009,23 +1210,23 @@
       <c r="A13" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="25">
-        <f t="shared" si="0"/>
-        <v>44854</v>
-      </c>
-      <c r="D13" s="26">
+      <c r="C13" s="11">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="D13" s="12">
         <v>0.66666666666666663</v>
       </c>
-      <c r="E13" s="23">
+      <c r="E13" s="3">
         <v>50</v>
       </c>
-      <c r="F13" s="23">
+      <c r="F13" s="3">
         <v>10</v>
       </c>
-      <c r="G13" s="23" t="s">
+      <c r="G13" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H13" s="13">
@@ -1036,23 +1237,23 @@
       <c r="A14" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="25">
-        <f t="shared" si="0"/>
-        <v>44854</v>
-      </c>
-      <c r="D14" s="26">
+      <c r="C14" s="11">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="D14" s="12">
         <v>0.75</v>
       </c>
-      <c r="E14" s="23">
+      <c r="E14" s="3">
         <v>50</v>
       </c>
-      <c r="F14" s="23">
+      <c r="F14" s="3">
         <v>23</v>
       </c>
-      <c r="G14" s="23" t="s">
+      <c r="G14" s="3" t="s">
         <v>17</v>
       </c>
       <c r="H14" s="13">
@@ -1063,23 +1264,23 @@
       <c r="A15" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="25">
-        <f t="shared" si="0"/>
-        <v>44854</v>
-      </c>
-      <c r="D15" s="26">
+      <c r="C15" s="11">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="D15" s="12">
         <v>0.83333333333333337</v>
       </c>
-      <c r="E15" s="23">
+      <c r="E15" s="3">
         <v>50</v>
       </c>
-      <c r="F15" s="23">
+      <c r="F15" s="3">
         <v>25</v>
       </c>
-      <c r="G15" s="23" t="s">
+      <c r="G15" s="3" t="s">
         <v>18</v>
       </c>
       <c r="H15" s="13">
@@ -1091,7 +1292,7 @@
         <v>29</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="C16" s="6">
         <f t="shared" si="0"/>
@@ -1117,24 +1318,24 @@
       <c r="A17" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="25">
-        <f t="shared" si="0"/>
-        <v>44854</v>
-      </c>
-      <c r="D17" s="26">
+      <c r="B17" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="11">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="D17" s="12">
         <f>D16+2*(1/24)</f>
         <v>0.41666666666666663</v>
       </c>
-      <c r="E17" s="23">
-        <v>20</v>
-      </c>
-      <c r="F17" s="23">
-        <v>29</v>
-      </c>
-      <c r="G17" s="23" t="s">
+      <c r="E17" s="3">
+        <v>20</v>
+      </c>
+      <c r="F17" s="3">
+        <v>29</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>20</v>
       </c>
       <c r="H17" s="13">
@@ -1145,24 +1346,24 @@
       <c r="A18" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="25">
-        <f t="shared" si="0"/>
-        <v>44854</v>
-      </c>
-      <c r="D18" s="26">
+      <c r="B18" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="11">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="D18" s="12">
         <f t="shared" si="1"/>
         <v>0.49999999999999994</v>
       </c>
-      <c r="E18" s="23">
-        <v>20</v>
-      </c>
-      <c r="F18" s="23">
-        <v>20</v>
-      </c>
-      <c r="G18" s="23" t="s">
+      <c r="E18" s="3">
+        <v>20</v>
+      </c>
+      <c r="F18" s="3">
+        <v>20</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>21</v>
       </c>
       <c r="H18" s="13">
@@ -1173,24 +1374,24 @@
       <c r="A19" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19" s="25">
-        <f t="shared" si="0"/>
-        <v>44854</v>
-      </c>
-      <c r="D19" s="26">
+      <c r="B19" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="11">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="D19" s="12">
         <f t="shared" si="1"/>
         <v>0.58333333333333326</v>
       </c>
-      <c r="E19" s="23">
-        <v>20</v>
-      </c>
-      <c r="F19" s="23">
+      <c r="E19" s="3">
+        <v>20</v>
+      </c>
+      <c r="F19" s="3">
         <v>16</v>
       </c>
-      <c r="G19" s="23" t="s">
+      <c r="G19" s="3" t="s">
         <v>22</v>
       </c>
       <c r="H19" s="13">
@@ -1201,24 +1402,24 @@
       <c r="A20" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20" s="25">
-        <f t="shared" si="0"/>
-        <v>44854</v>
-      </c>
-      <c r="D20" s="26">
+      <c r="B20" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="11">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="D20" s="12">
         <f t="shared" si="1"/>
         <v>0.66666666666666663</v>
       </c>
-      <c r="E20" s="23">
-        <v>20</v>
-      </c>
-      <c r="F20" s="23">
+      <c r="E20" s="3">
+        <v>20</v>
+      </c>
+      <c r="F20" s="3">
         <v>24</v>
       </c>
-      <c r="G20" s="23" t="s">
+      <c r="G20" s="3" t="s">
         <v>23</v>
       </c>
       <c r="H20" s="13">
@@ -1229,24 +1430,24 @@
       <c r="A21" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" s="25">
-        <f t="shared" si="0"/>
-        <v>44854</v>
-      </c>
-      <c r="D21" s="26">
+      <c r="B21" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="11">
+        <f t="shared" si="0"/>
+        <v>44854</v>
+      </c>
+      <c r="D21" s="12">
         <f t="shared" si="1"/>
         <v>0.75</v>
       </c>
-      <c r="E21" s="23">
-        <v>20</v>
-      </c>
-      <c r="F21" s="23">
+      <c r="E21" s="3">
+        <v>20</v>
+      </c>
+      <c r="F21" s="3">
         <v>27</v>
       </c>
-      <c r="G21" s="23" t="s">
+      <c r="G21" s="3" t="s">
         <v>24</v>
       </c>
       <c r="H21" s="13">
@@ -1258,7 +1459,7 @@
         <v>29</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="C22" s="15">
         <f t="shared" si="0"/>
@@ -1282,7 +1483,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="24" t="s">
+      <c r="A24" s="23" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1292,7 +1493,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C4ED15D-191C-4AAB-A5B7-A6DBCC742E4E}">
   <dimension ref="A1:L43"/>
   <sheetViews>
@@ -1984,7 +2185,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9E57897-8241-456F-B820-85D5C0044E1A}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>